<commit_message>
Turkey's Unit Value added to Data Files
</commit_message>
<xml_diff>
--- a/Data_Sources_and_Preparation/ITC_Trade_Data/841810_GBR_all_unit_value.xlsx
+++ b/Data_Sources_and_Preparation/ITC_Trade_Data/841810_GBR_all_unit_value.xlsx
@@ -16,10 +16,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>Date</t>
+    <t>TUR_GBR_841810_UV</t>
   </si>
   <si>
-    <t>TUR_GBR_841810_UV</t>
+    <t>Date</t>
   </si>
   <si>
     <t>TUR_GBR_841810_UV-1</t>
@@ -422,44 +422,44 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2">
+      <c r="B2">
         <v>200404</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3">
+      <c r="B3">
         <v>200405</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4">
+      <c r="B4">
         <v>200406</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5">
+      <c r="B5">
         <v>200407</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6">
+      <c r="B6">
         <v>200408</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7">
+        <v>16</v>
+      </c>
+      <c r="B7">
         <v>200409</v>
-      </c>
-      <c r="B7">
-        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8">
         <v>200410</v>
-      </c>
-      <c r="B8">
-        <v>10</v>
       </c>
       <c r="C8">
         <v>16</v>
@@ -467,10 +467,10 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9">
+        <v>4.67</v>
+      </c>
+      <c r="B9">
         <v>200411</v>
-      </c>
-      <c r="B9">
-        <v>4.67</v>
       </c>
       <c r="C9">
         <v>10</v>
@@ -480,7 +480,7 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10">
+      <c r="B10">
         <v>200412</v>
       </c>
       <c r="C10">
@@ -494,7 +494,7 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11">
+      <c r="B11">
         <v>200501</v>
       </c>
       <c r="D11">
@@ -506,17 +506,17 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12">
+        <v>6.36</v>
+      </c>
+      <c r="B12">
         <v>200502</v>
-      </c>
-      <c r="B12">
-        <v>6.36</v>
       </c>
       <c r="E12">
         <v>4.67</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13">
+      <c r="B13">
         <v>200503</v>
       </c>
       <c r="C13">
@@ -527,7 +527,7 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14">
+      <c r="B14">
         <v>200504</v>
       </c>
       <c r="D14">
@@ -539,10 +539,10 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15">
+        <v>5.49</v>
+      </c>
+      <c r="B15">
         <v>200505</v>
-      </c>
-      <c r="B15">
-        <v>5.49</v>
       </c>
       <c r="E15">
         <v>6.36</v>
@@ -552,7 +552,7 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16">
+      <c r="B16">
         <v>200506</v>
       </c>
       <c r="C16">
@@ -560,7 +560,7 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17">
+      <c r="B17">
         <v>200507</v>
       </c>
       <c r="D17">
@@ -568,7 +568,7 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18">
+      <c r="B18">
         <v>200508</v>
       </c>
       <c r="E18">
@@ -579,7 +579,7 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19">
+      <c r="B19">
         <v>200509</v>
       </c>
       <c r="G19">
@@ -587,7 +587,7 @@
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20">
+      <c r="B20">
         <v>200510</v>
       </c>
       <c r="G20">
@@ -595,7 +595,7 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21">
+      <c r="B21">
         <v>200511</v>
       </c>
       <c r="F21">
@@ -606,28 +606,28 @@
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22">
+      <c r="B22">
         <v>200512</v>
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23">
+      <c r="B23">
         <v>200601</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24">
+        <v>13</v>
+      </c>
+      <c r="B24">
         <v>200602</v>
-      </c>
-      <c r="B24">
-        <v>13</v>
       </c>
       <c r="G24">
         <v>6.36</v>
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25">
+      <c r="B25">
         <v>200603</v>
       </c>
       <c r="C25">
@@ -635,7 +635,7 @@
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26">
+      <c r="B26">
         <v>200604</v>
       </c>
       <c r="D26">
@@ -643,7 +643,7 @@
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27">
+      <c r="B27">
         <v>200605</v>
       </c>
       <c r="E27">
@@ -655,18 +655,18 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28">
+        <v>3.76</v>
+      </c>
+      <c r="B28">
         <v>200606</v>
-      </c>
-      <c r="B28">
-        <v>3.76</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29">
+        <v>3.96</v>
+      </c>
+      <c r="B29">
         <v>200607</v>
-      </c>
-      <c r="B29">
-        <v>3.96</v>
       </c>
       <c r="C29">
         <v>3.76</v>
@@ -674,10 +674,10 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30">
+        <v>3.96</v>
+      </c>
+      <c r="B30">
         <v>200608</v>
-      </c>
-      <c r="B30">
-        <v>3.96</v>
       </c>
       <c r="C30">
         <v>3.96</v>
@@ -691,10 +691,10 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31">
+        <v>4.3</v>
+      </c>
+      <c r="B31">
         <v>200609</v>
-      </c>
-      <c r="B31">
-        <v>4.3</v>
       </c>
       <c r="C31">
         <v>3.96</v>
@@ -708,10 +708,10 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32">
+        <v>4.74</v>
+      </c>
+      <c r="B32">
         <v>200610</v>
-      </c>
-      <c r="B32">
-        <v>4.74</v>
       </c>
       <c r="C32">
         <v>4.3</v>
@@ -725,10 +725,10 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33">
+        <v>3.82</v>
+      </c>
+      <c r="B33">
         <v>200611</v>
-      </c>
-      <c r="B33">
-        <v>3.82</v>
       </c>
       <c r="C33">
         <v>4.74</v>
@@ -742,10 +742,10 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34">
+        <v>3.91</v>
+      </c>
+      <c r="B34">
         <v>200612</v>
-      </c>
-      <c r="B34">
-        <v>3.91</v>
       </c>
       <c r="C34">
         <v>3.82</v>
@@ -762,10 +762,10 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35">
+        <v>3.94</v>
+      </c>
+      <c r="B35">
         <v>200701</v>
-      </c>
-      <c r="B35">
-        <v>3.94</v>
       </c>
       <c r="C35">
         <v>3.91</v>
@@ -782,10 +782,10 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36">
+        <v>3.79</v>
+      </c>
+      <c r="B36">
         <v>200702</v>
-      </c>
-      <c r="B36">
-        <v>3.79</v>
       </c>
       <c r="C36">
         <v>3.94</v>
@@ -805,10 +805,10 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37">
+        <v>4.34</v>
+      </c>
+      <c r="B37">
         <v>200703</v>
-      </c>
-      <c r="B37">
-        <v>4.34</v>
       </c>
       <c r="C37">
         <v>3.79</v>
@@ -825,10 +825,10 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38">
+        <v>4.55</v>
+      </c>
+      <c r="B38">
         <v>200704</v>
-      </c>
-      <c r="B38">
-        <v>4.55</v>
       </c>
       <c r="C38">
         <v>4.34</v>
@@ -845,10 +845,10 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39">
+        <v>4.43</v>
+      </c>
+      <c r="B39">
         <v>200705</v>
-      </c>
-      <c r="B39">
-        <v>4.43</v>
       </c>
       <c r="C39">
         <v>4.55</v>
@@ -865,10 +865,10 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40">
+        <v>4.35</v>
+      </c>
+      <c r="B40">
         <v>200706</v>
-      </c>
-      <c r="B40">
-        <v>4.35</v>
       </c>
       <c r="C40">
         <v>4.43</v>
@@ -888,10 +888,10 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41">
+        <v>4.34</v>
+      </c>
+      <c r="B41">
         <v>200707</v>
-      </c>
-      <c r="B41">
-        <v>4.34</v>
       </c>
       <c r="C41">
         <v>4.35</v>
@@ -911,10 +911,10 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42">
+        <v>4.18</v>
+      </c>
+      <c r="B42">
         <v>200708</v>
-      </c>
-      <c r="B42">
-        <v>4.18</v>
       </c>
       <c r="C42">
         <v>4.34</v>
@@ -934,10 +934,10 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43">
+        <v>4.36</v>
+      </c>
+      <c r="B43">
         <v>200709</v>
-      </c>
-      <c r="B43">
-        <v>4.36</v>
       </c>
       <c r="C43">
         <v>4.18</v>
@@ -957,10 +957,10 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44">
+        <v>4.61</v>
+      </c>
+      <c r="B44">
         <v>200710</v>
-      </c>
-      <c r="B44">
-        <v>4.61</v>
       </c>
       <c r="C44">
         <v>4.36</v>
@@ -980,10 +980,10 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45">
+        <v>4.6</v>
+      </c>
+      <c r="B45">
         <v>200711</v>
-      </c>
-      <c r="B45">
-        <v>4.6</v>
       </c>
       <c r="C45">
         <v>4.61</v>
@@ -1003,10 +1003,10 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46">
+        <v>4.36</v>
+      </c>
+      <c r="B46">
         <v>200712</v>
-      </c>
-      <c r="B46">
-        <v>4.36</v>
       </c>
       <c r="C46">
         <v>4.6</v>
@@ -1026,10 +1026,10 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47">
+        <v>4.39</v>
+      </c>
+      <c r="B47">
         <v>200801</v>
-      </c>
-      <c r="B47">
-        <v>4.39</v>
       </c>
       <c r="C47">
         <v>4.36</v>
@@ -1049,10 +1049,10 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48">
+        <v>4.33</v>
+      </c>
+      <c r="B48">
         <v>200802</v>
-      </c>
-      <c r="B48">
-        <v>4.33</v>
       </c>
       <c r="C48">
         <v>4.39</v>
@@ -1072,10 +1072,10 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49">
+        <v>4.36</v>
+      </c>
+      <c r="B49">
         <v>200803</v>
-      </c>
-      <c r="B49">
-        <v>4.36</v>
       </c>
       <c r="C49">
         <v>4.33</v>
@@ -1095,10 +1095,10 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50">
+        <v>4.1</v>
+      </c>
+      <c r="B50">
         <v>200804</v>
-      </c>
-      <c r="B50">
-        <v>4.1</v>
       </c>
       <c r="C50">
         <v>4.36</v>
@@ -1118,10 +1118,10 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51">
+        <v>4.24</v>
+      </c>
+      <c r="B51">
         <v>200805</v>
-      </c>
-      <c r="B51">
-        <v>4.24</v>
       </c>
       <c r="C51">
         <v>4.1</v>
@@ -1141,10 +1141,10 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52">
+        <v>4.42</v>
+      </c>
+      <c r="B52">
         <v>200806</v>
-      </c>
-      <c r="B52">
-        <v>4.42</v>
       </c>
       <c r="C52">
         <v>4.24</v>
@@ -1164,10 +1164,10 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53">
+        <v>4.32</v>
+      </c>
+      <c r="B53">
         <v>200807</v>
-      </c>
-      <c r="B53">
-        <v>4.32</v>
       </c>
       <c r="C53">
         <v>4.42</v>
@@ -1187,10 +1187,10 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54">
+        <v>4.31</v>
+      </c>
+      <c r="B54">
         <v>200808</v>
-      </c>
-      <c r="B54">
-        <v>4.31</v>
       </c>
       <c r="C54">
         <v>4.32</v>
@@ -1210,10 +1210,10 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55">
+        <v>3.88</v>
+      </c>
+      <c r="B55">
         <v>200809</v>
-      </c>
-      <c r="B55">
-        <v>3.88</v>
       </c>
       <c r="C55">
         <v>4.31</v>
@@ -1233,10 +1233,10 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56">
+        <v>3.43</v>
+      </c>
+      <c r="B56">
         <v>200810</v>
-      </c>
-      <c r="B56">
-        <v>3.43</v>
       </c>
       <c r="C56">
         <v>3.88</v>
@@ -1256,10 +1256,10 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57">
+        <v>3.26</v>
+      </c>
+      <c r="B57">
         <v>200811</v>
-      </c>
-      <c r="B57">
-        <v>3.26</v>
       </c>
       <c r="C57">
         <v>3.43</v>
@@ -1279,10 +1279,10 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58">
+        <v>3.19</v>
+      </c>
+      <c r="B58">
         <v>200812</v>
-      </c>
-      <c r="B58">
-        <v>3.19</v>
       </c>
       <c r="C58">
         <v>3.26</v>
@@ -1302,10 +1302,10 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59">
+        <v>3.15</v>
+      </c>
+      <c r="B59">
         <v>200901</v>
-      </c>
-      <c r="B59">
-        <v>3.15</v>
       </c>
       <c r="C59">
         <v>3.19</v>
@@ -1325,10 +1325,10 @@
     </row>
     <row r="60" spans="1:7">
       <c r="A60">
+        <v>3.43</v>
+      </c>
+      <c r="B60">
         <v>200902</v>
-      </c>
-      <c r="B60">
-        <v>3.43</v>
       </c>
       <c r="C60">
         <v>3.15</v>
@@ -1348,10 +1348,10 @@
     </row>
     <row r="61" spans="1:7">
       <c r="A61">
+        <v>3.25</v>
+      </c>
+      <c r="B61">
         <v>200903</v>
-      </c>
-      <c r="B61">
-        <v>3.25</v>
       </c>
       <c r="C61">
         <v>3.43</v>
@@ -1371,10 +1371,10 @@
     </row>
     <row r="62" spans="1:7">
       <c r="A62">
+        <v>3.09</v>
+      </c>
+      <c r="B62">
         <v>200904</v>
-      </c>
-      <c r="B62">
-        <v>3.09</v>
       </c>
       <c r="C62">
         <v>3.25</v>
@@ -1394,10 +1394,10 @@
     </row>
     <row r="63" spans="1:7">
       <c r="A63">
+        <v>3.27</v>
+      </c>
+      <c r="B63">
         <v>200905</v>
-      </c>
-      <c r="B63">
-        <v>3.27</v>
       </c>
       <c r="C63">
         <v>3.09</v>
@@ -1417,10 +1417,10 @@
     </row>
     <row r="64" spans="1:7">
       <c r="A64">
+        <v>3.48</v>
+      </c>
+      <c r="B64">
         <v>200906</v>
-      </c>
-      <c r="B64">
-        <v>3.48</v>
       </c>
       <c r="C64">
         <v>3.27</v>
@@ -1440,10 +1440,10 @@
     </row>
     <row r="65" spans="1:7">
       <c r="A65">
+        <v>3.53</v>
+      </c>
+      <c r="B65">
         <v>200907</v>
-      </c>
-      <c r="B65">
-        <v>3.53</v>
       </c>
       <c r="C65">
         <v>3.48</v>
@@ -1463,10 +1463,10 @@
     </row>
     <row r="66" spans="1:7">
       <c r="A66">
+        <v>3.49</v>
+      </c>
+      <c r="B66">
         <v>200908</v>
-      </c>
-      <c r="B66">
-        <v>3.49</v>
       </c>
       <c r="C66">
         <v>3.53</v>
@@ -1486,10 +1486,10 @@
     </row>
     <row r="67" spans="1:7">
       <c r="A67">
+        <v>3.5</v>
+      </c>
+      <c r="B67">
         <v>200909</v>
-      </c>
-      <c r="B67">
-        <v>3.5</v>
       </c>
       <c r="C67">
         <v>3.49</v>
@@ -1509,10 +1509,10 @@
     </row>
     <row r="68" spans="1:7">
       <c r="A68">
+        <v>3.45</v>
+      </c>
+      <c r="B68">
         <v>200910</v>
-      </c>
-      <c r="B68">
-        <v>3.45</v>
       </c>
       <c r="C68">
         <v>3.5</v>
@@ -1532,10 +1532,10 @@
     </row>
     <row r="69" spans="1:7">
       <c r="A69">
+        <v>3.58</v>
+      </c>
+      <c r="B69">
         <v>200911</v>
-      </c>
-      <c r="B69">
-        <v>3.58</v>
       </c>
       <c r="C69">
         <v>3.45</v>
@@ -1555,10 +1555,10 @@
     </row>
     <row r="70" spans="1:7">
       <c r="A70">
+        <v>3.62</v>
+      </c>
+      <c r="B70">
         <v>200912</v>
-      </c>
-      <c r="B70">
-        <v>3.62</v>
       </c>
       <c r="C70">
         <v>3.58</v>
@@ -1578,10 +1578,10 @@
     </row>
     <row r="71" spans="1:7">
       <c r="A71">
+        <v>3.61</v>
+      </c>
+      <c r="B71">
         <v>201001</v>
-      </c>
-      <c r="B71">
-        <v>3.61</v>
       </c>
       <c r="C71">
         <v>3.62</v>
@@ -1601,10 +1601,10 @@
     </row>
     <row r="72" spans="1:7">
       <c r="A72">
+        <v>3.46</v>
+      </c>
+      <c r="B72">
         <v>201002</v>
-      </c>
-      <c r="B72">
-        <v>3.46</v>
       </c>
       <c r="C72">
         <v>3.61</v>
@@ -1624,10 +1624,10 @@
     </row>
     <row r="73" spans="1:7">
       <c r="A73">
+        <v>3.31</v>
+      </c>
+      <c r="B73">
         <v>201003</v>
-      </c>
-      <c r="B73">
-        <v>3.31</v>
       </c>
       <c r="C73">
         <v>3.46</v>
@@ -1647,10 +1647,10 @@
     </row>
     <row r="74" spans="1:7">
       <c r="A74">
+        <v>3.36</v>
+      </c>
+      <c r="B74">
         <v>201004</v>
-      </c>
-      <c r="B74">
-        <v>3.36</v>
       </c>
       <c r="C74">
         <v>3.31</v>
@@ -1670,10 +1670,10 @@
     </row>
     <row r="75" spans="1:7">
       <c r="A75">
+        <v>3.26</v>
+      </c>
+      <c r="B75">
         <v>201005</v>
-      </c>
-      <c r="B75">
-        <v>3.26</v>
       </c>
       <c r="C75">
         <v>3.36</v>
@@ -1693,10 +1693,10 @@
     </row>
     <row r="76" spans="1:7">
       <c r="A76">
+        <v>3.22</v>
+      </c>
+      <c r="B76">
         <v>201006</v>
-      </c>
-      <c r="B76">
-        <v>3.22</v>
       </c>
       <c r="C76">
         <v>3.26</v>
@@ -1716,10 +1716,10 @@
     </row>
     <row r="77" spans="1:7">
       <c r="A77">
+        <v>3.29</v>
+      </c>
+      <c r="B77">
         <v>201007</v>
-      </c>
-      <c r="B77">
-        <v>3.29</v>
       </c>
       <c r="C77">
         <v>3.22</v>
@@ -1739,10 +1739,10 @@
     </row>
     <row r="78" spans="1:7">
       <c r="A78">
+        <v>3.46</v>
+      </c>
+      <c r="B78">
         <v>201008</v>
-      </c>
-      <c r="B78">
-        <v>3.46</v>
       </c>
       <c r="C78">
         <v>3.29</v>
@@ -1762,10 +1762,10 @@
     </row>
     <row r="79" spans="1:7">
       <c r="A79">
+        <v>3.39</v>
+      </c>
+      <c r="B79">
         <v>201009</v>
-      </c>
-      <c r="B79">
-        <v>3.39</v>
       </c>
       <c r="C79">
         <v>3.46</v>
@@ -1785,10 +1785,10 @@
     </row>
     <row r="80" spans="1:7">
       <c r="A80">
+        <v>3.56</v>
+      </c>
+      <c r="B80">
         <v>201010</v>
-      </c>
-      <c r="B80">
-        <v>3.56</v>
       </c>
       <c r="C80">
         <v>3.39</v>
@@ -1808,10 +1808,10 @@
     </row>
     <row r="81" spans="1:7">
       <c r="A81">
+        <v>3.53</v>
+      </c>
+      <c r="B81">
         <v>201011</v>
-      </c>
-      <c r="B81">
-        <v>3.53</v>
       </c>
       <c r="C81">
         <v>3.56</v>
@@ -1831,10 +1831,10 @@
     </row>
     <row r="82" spans="1:7">
       <c r="A82">
+        <v>3.47</v>
+      </c>
+      <c r="B82">
         <v>201012</v>
-      </c>
-      <c r="B82">
-        <v>3.47</v>
       </c>
       <c r="C82">
         <v>3.53</v>
@@ -1854,10 +1854,10 @@
     </row>
     <row r="83" spans="1:7">
       <c r="A83">
+        <v>3.66</v>
+      </c>
+      <c r="B83">
         <v>201101</v>
-      </c>
-      <c r="B83">
-        <v>3.66</v>
       </c>
       <c r="C83">
         <v>3.47</v>
@@ -1877,10 +1877,10 @@
     </row>
     <row r="84" spans="1:7">
       <c r="A84">
+        <v>3.67</v>
+      </c>
+      <c r="B84">
         <v>201102</v>
-      </c>
-      <c r="B84">
-        <v>3.67</v>
       </c>
       <c r="C84">
         <v>3.66</v>
@@ -1900,10 +1900,10 @@
     </row>
     <row r="85" spans="1:7">
       <c r="A85">
+        <v>3.63</v>
+      </c>
+      <c r="B85">
         <v>201103</v>
-      </c>
-      <c r="B85">
-        <v>3.63</v>
       </c>
       <c r="C85">
         <v>3.67</v>
@@ -1923,10 +1923,10 @@
     </row>
     <row r="86" spans="1:7">
       <c r="A86">
+        <v>3.78</v>
+      </c>
+      <c r="B86">
         <v>201104</v>
-      </c>
-      <c r="B86">
-        <v>3.78</v>
       </c>
       <c r="C86">
         <v>3.63</v>
@@ -1946,10 +1946,10 @@
     </row>
     <row r="87" spans="1:7">
       <c r="A87">
+        <v>3.71</v>
+      </c>
+      <c r="B87">
         <v>201105</v>
-      </c>
-      <c r="B87">
-        <v>3.71</v>
       </c>
       <c r="C87">
         <v>3.78</v>
@@ -1969,10 +1969,10 @@
     </row>
     <row r="88" spans="1:7">
       <c r="A88">
+        <v>4.05</v>
+      </c>
+      <c r="B88">
         <v>201106</v>
-      </c>
-      <c r="B88">
-        <v>4.05</v>
       </c>
       <c r="C88">
         <v>3.71</v>
@@ -1992,10 +1992,10 @@
     </row>
     <row r="89" spans="1:7">
       <c r="A89">
+        <v>3.83</v>
+      </c>
+      <c r="B89">
         <v>201107</v>
-      </c>
-      <c r="B89">
-        <v>3.83</v>
       </c>
       <c r="C89">
         <v>4.05</v>
@@ -2015,10 +2015,10 @@
     </row>
     <row r="90" spans="1:7">
       <c r="A90">
+        <v>3.78</v>
+      </c>
+      <c r="B90">
         <v>201108</v>
-      </c>
-      <c r="B90">
-        <v>3.78</v>
       </c>
       <c r="C90">
         <v>3.83</v>
@@ -2038,10 +2038,10 @@
     </row>
     <row r="91" spans="1:7">
       <c r="A91">
+        <v>3.54</v>
+      </c>
+      <c r="B91">
         <v>201109</v>
-      </c>
-      <c r="B91">
-        <v>3.54</v>
       </c>
       <c r="C91">
         <v>3.78</v>
@@ -2061,10 +2061,10 @@
     </row>
     <row r="92" spans="1:7">
       <c r="A92">
+        <v>3.56</v>
+      </c>
+      <c r="B92">
         <v>201110</v>
-      </c>
-      <c r="B92">
-        <v>3.56</v>
       </c>
       <c r="C92">
         <v>3.54</v>
@@ -2084,10 +2084,10 @@
     </row>
     <row r="93" spans="1:7">
       <c r="A93">
+        <v>3.5</v>
+      </c>
+      <c r="B93">
         <v>201111</v>
-      </c>
-      <c r="B93">
-        <v>3.5</v>
       </c>
       <c r="C93">
         <v>3.56</v>
@@ -2107,10 +2107,10 @@
     </row>
     <row r="94" spans="1:7">
       <c r="A94">
+        <v>3.42</v>
+      </c>
+      <c r="B94">
         <v>201112</v>
-      </c>
-      <c r="B94">
-        <v>3.42</v>
       </c>
       <c r="C94">
         <v>3.5</v>
@@ -2130,10 +2130,10 @@
     </row>
     <row r="95" spans="1:7">
       <c r="A95">
+        <v>3.47</v>
+      </c>
+      <c r="B95">
         <v>201201</v>
-      </c>
-      <c r="B95">
-        <v>3.47</v>
       </c>
       <c r="C95">
         <v>3.42</v>
@@ -2153,10 +2153,10 @@
     </row>
     <row r="96" spans="1:7">
       <c r="A96">
+        <v>3.53</v>
+      </c>
+      <c r="B96">
         <v>201202</v>
-      </c>
-      <c r="B96">
-        <v>3.53</v>
       </c>
       <c r="C96">
         <v>3.47</v>
@@ -2176,10 +2176,10 @@
     </row>
     <row r="97" spans="1:7">
       <c r="A97">
+        <v>3.5</v>
+      </c>
+      <c r="B97">
         <v>201203</v>
-      </c>
-      <c r="B97">
-        <v>3.5</v>
       </c>
       <c r="C97">
         <v>3.53</v>
@@ -2199,10 +2199,10 @@
     </row>
     <row r="98" spans="1:7">
       <c r="A98">
+        <v>3.47</v>
+      </c>
+      <c r="B98">
         <v>201204</v>
-      </c>
-      <c r="B98">
-        <v>3.47</v>
       </c>
       <c r="C98">
         <v>3.5</v>
@@ -2222,10 +2222,10 @@
     </row>
     <row r="99" spans="1:7">
       <c r="A99">
+        <v>3.63</v>
+      </c>
+      <c r="B99">
         <v>201205</v>
-      </c>
-      <c r="B99">
-        <v>3.63</v>
       </c>
       <c r="C99">
         <v>3.47</v>
@@ -2245,10 +2245,10 @@
     </row>
     <row r="100" spans="1:7">
       <c r="A100">
+        <v>3.61</v>
+      </c>
+      <c r="B100">
         <v>201206</v>
-      </c>
-      <c r="B100">
-        <v>3.61</v>
       </c>
       <c r="C100">
         <v>3.63</v>
@@ -2268,10 +2268,10 @@
     </row>
     <row r="101" spans="1:7">
       <c r="A101">
+        <v>3.53</v>
+      </c>
+      <c r="B101">
         <v>201207</v>
-      </c>
-      <c r="B101">
-        <v>3.53</v>
       </c>
       <c r="C101">
         <v>3.61</v>
@@ -2291,10 +2291,10 @@
     </row>
     <row r="102" spans="1:7">
       <c r="A102">
+        <v>3.61</v>
+      </c>
+      <c r="B102">
         <v>201208</v>
-      </c>
-      <c r="B102">
-        <v>3.61</v>
       </c>
       <c r="C102">
         <v>3.53</v>
@@ -2314,10 +2314,10 @@
     </row>
     <row r="103" spans="1:7">
       <c r="A103">
+        <v>3.67</v>
+      </c>
+      <c r="B103">
         <v>201209</v>
-      </c>
-      <c r="B103">
-        <v>3.67</v>
       </c>
       <c r="C103">
         <v>3.61</v>
@@ -2337,10 +2337,10 @@
     </row>
     <row r="104" spans="1:7">
       <c r="A104">
+        <v>3.65</v>
+      </c>
+      <c r="B104">
         <v>201210</v>
-      </c>
-      <c r="B104">
-        <v>3.65</v>
       </c>
       <c r="C104">
         <v>3.67</v>
@@ -2360,10 +2360,10 @@
     </row>
     <row r="105" spans="1:7">
       <c r="A105">
+        <v>3.69</v>
+      </c>
+      <c r="B105">
         <v>201211</v>
-      </c>
-      <c r="B105">
-        <v>3.69</v>
       </c>
       <c r="C105">
         <v>3.65</v>
@@ -2383,10 +2383,10 @@
     </row>
     <row r="106" spans="1:7">
       <c r="A106">
+        <v>3.61</v>
+      </c>
+      <c r="B106">
         <v>201212</v>
-      </c>
-      <c r="B106">
-        <v>3.61</v>
       </c>
       <c r="C106">
         <v>3.69</v>
@@ -2406,10 +2406,10 @@
     </row>
     <row r="107" spans="1:7">
       <c r="A107">
+        <v>3.72</v>
+      </c>
+      <c r="B107">
         <v>201301</v>
-      </c>
-      <c r="B107">
-        <v>3.72</v>
       </c>
       <c r="C107">
         <v>3.61</v>
@@ -2429,10 +2429,10 @@
     </row>
     <row r="108" spans="1:7">
       <c r="A108">
+        <v>3.81</v>
+      </c>
+      <c r="B108">
         <v>201302</v>
-      </c>
-      <c r="B108">
-        <v>3.81</v>
       </c>
       <c r="C108">
         <v>3.72</v>
@@ -2452,10 +2452,10 @@
     </row>
     <row r="109" spans="1:7">
       <c r="A109">
+        <v>3.61</v>
+      </c>
+      <c r="B109">
         <v>201303</v>
-      </c>
-      <c r="B109">
-        <v>3.61</v>
       </c>
       <c r="C109">
         <v>3.81</v>
@@ -2475,10 +2475,10 @@
     </row>
     <row r="110" spans="1:7">
       <c r="A110">
+        <v>3.68</v>
+      </c>
+      <c r="B110">
         <v>201304</v>
-      </c>
-      <c r="B110">
-        <v>3.68</v>
       </c>
       <c r="C110">
         <v>3.61</v>
@@ -2498,10 +2498,10 @@
     </row>
     <row r="111" spans="1:7">
       <c r="A111">
+        <v>3.67</v>
+      </c>
+      <c r="B111">
         <v>201305</v>
-      </c>
-      <c r="B111">
-        <v>3.67</v>
       </c>
       <c r="C111">
         <v>3.68</v>
@@ -2521,10 +2521,10 @@
     </row>
     <row r="112" spans="1:7">
       <c r="A112">
+        <v>3.76</v>
+      </c>
+      <c r="B112">
         <v>201306</v>
-      </c>
-      <c r="B112">
-        <v>3.76</v>
       </c>
       <c r="C112">
         <v>3.67</v>
@@ -2544,10 +2544,10 @@
     </row>
     <row r="113" spans="1:7">
       <c r="A113">
+        <v>3.63</v>
+      </c>
+      <c r="B113">
         <v>201307</v>
-      </c>
-      <c r="B113">
-        <v>3.63</v>
       </c>
       <c r="C113">
         <v>3.76</v>
@@ -2567,10 +2567,10 @@
     </row>
     <row r="114" spans="1:7">
       <c r="A114">
+        <v>3.65</v>
+      </c>
+      <c r="B114">
         <v>201308</v>
-      </c>
-      <c r="B114">
-        <v>3.65</v>
       </c>
       <c r="C114">
         <v>3.63</v>
@@ -2590,10 +2590,10 @@
     </row>
     <row r="115" spans="1:7">
       <c r="A115">
+        <v>3.66</v>
+      </c>
+      <c r="B115">
         <v>201309</v>
-      </c>
-      <c r="B115">
-        <v>3.66</v>
       </c>
       <c r="C115">
         <v>3.65</v>
@@ -2613,10 +2613,10 @@
     </row>
     <row r="116" spans="1:7">
       <c r="A116">
+        <v>3.6</v>
+      </c>
+      <c r="B116">
         <v>201310</v>
-      </c>
-      <c r="B116">
-        <v>3.6</v>
       </c>
       <c r="C116">
         <v>3.66</v>
@@ -2636,10 +2636,10 @@
     </row>
     <row r="117" spans="1:7">
       <c r="A117">
+        <v>3.54</v>
+      </c>
+      <c r="B117">
         <v>201311</v>
-      </c>
-      <c r="B117">
-        <v>3.54</v>
       </c>
       <c r="C117">
         <v>3.6</v>
@@ -2659,10 +2659,10 @@
     </row>
     <row r="118" spans="1:7">
       <c r="A118">
+        <v>3.53</v>
+      </c>
+      <c r="B118">
         <v>201312</v>
-      </c>
-      <c r="B118">
-        <v>3.53</v>
       </c>
       <c r="C118">
         <v>3.54</v>
@@ -2682,10 +2682,10 @@
     </row>
     <row r="119" spans="1:7">
       <c r="A119">
+        <v>3.71</v>
+      </c>
+      <c r="B119">
         <v>201401</v>
-      </c>
-      <c r="B119">
-        <v>3.71</v>
       </c>
       <c r="C119">
         <v>3.53</v>
@@ -2705,10 +2705,10 @@
     </row>
     <row r="120" spans="1:7">
       <c r="A120">
+        <v>3.69</v>
+      </c>
+      <c r="B120">
         <v>201402</v>
-      </c>
-      <c r="B120">
-        <v>3.69</v>
       </c>
       <c r="C120">
         <v>3.71</v>
@@ -2728,10 +2728,10 @@
     </row>
     <row r="121" spans="1:7">
       <c r="A121">
+        <v>3.78</v>
+      </c>
+      <c r="B121">
         <v>201403</v>
-      </c>
-      <c r="B121">
-        <v>3.78</v>
       </c>
       <c r="C121">
         <v>3.69</v>
@@ -2751,10 +2751,10 @@
     </row>
     <row r="122" spans="1:7">
       <c r="A122">
+        <v>3.83</v>
+      </c>
+      <c r="B122">
         <v>201404</v>
-      </c>
-      <c r="B122">
-        <v>3.83</v>
       </c>
       <c r="C122">
         <v>3.78</v>
@@ -2774,10 +2774,10 @@
     </row>
     <row r="123" spans="1:7">
       <c r="A123">
+        <v>3.98</v>
+      </c>
+      <c r="B123">
         <v>201405</v>
-      </c>
-      <c r="B123">
-        <v>3.98</v>
       </c>
       <c r="C123">
         <v>3.83</v>
@@ -2797,10 +2797,10 @@
     </row>
     <row r="124" spans="1:7">
       <c r="A124">
+        <v>3.97</v>
+      </c>
+      <c r="B124">
         <v>201406</v>
-      </c>
-      <c r="B124">
-        <v>3.97</v>
       </c>
       <c r="C124">
         <v>3.98</v>
@@ -2820,10 +2820,10 @@
     </row>
     <row r="125" spans="1:7">
       <c r="A125">
+        <v>4.01</v>
+      </c>
+      <c r="B125">
         <v>201407</v>
-      </c>
-      <c r="B125">
-        <v>4.01</v>
       </c>
       <c r="C125">
         <v>3.97</v>
@@ -2843,10 +2843,10 @@
     </row>
     <row r="126" spans="1:7">
       <c r="A126">
+        <v>3.87</v>
+      </c>
+      <c r="B126">
         <v>201408</v>
-      </c>
-      <c r="B126">
-        <v>3.87</v>
       </c>
       <c r="C126">
         <v>4.01</v>
@@ -2866,10 +2866,10 @@
     </row>
     <row r="127" spans="1:7">
       <c r="A127">
+        <v>3.75</v>
+      </c>
+      <c r="B127">
         <v>201409</v>
-      </c>
-      <c r="B127">
-        <v>3.75</v>
       </c>
       <c r="C127">
         <v>3.87</v>
@@ -2889,10 +2889,10 @@
     </row>
     <row r="128" spans="1:7">
       <c r="A128">
+        <v>3.67</v>
+      </c>
+      <c r="B128">
         <v>201410</v>
-      </c>
-      <c r="B128">
-        <v>3.67</v>
       </c>
       <c r="C128">
         <v>3.75</v>
@@ -2912,10 +2912,10 @@
     </row>
     <row r="129" spans="1:7">
       <c r="A129">
+        <v>3.54</v>
+      </c>
+      <c r="B129">
         <v>201411</v>
-      </c>
-      <c r="B129">
-        <v>3.54</v>
       </c>
       <c r="C129">
         <v>3.67</v>
@@ -2935,10 +2935,10 @@
     </row>
     <row r="130" spans="1:7">
       <c r="A130">
+        <v>3.4</v>
+      </c>
+      <c r="B130">
         <v>201412</v>
-      </c>
-      <c r="B130">
-        <v>3.4</v>
       </c>
       <c r="C130">
         <v>3.54</v>
@@ -2958,10 +2958,10 @@
     </row>
     <row r="131" spans="1:7">
       <c r="A131">
+        <v>3.38</v>
+      </c>
+      <c r="B131">
         <v>201501</v>
-      </c>
-      <c r="B131">
-        <v>3.38</v>
       </c>
       <c r="C131">
         <v>3.4</v>
@@ -2981,10 +2981,10 @@
     </row>
     <row r="132" spans="1:7">
       <c r="A132">
+        <v>3.29</v>
+      </c>
+      <c r="B132">
         <v>201502</v>
-      </c>
-      <c r="B132">
-        <v>3.29</v>
       </c>
       <c r="C132">
         <v>3.38</v>
@@ -3004,10 +3004,10 @@
     </row>
     <row r="133" spans="1:7">
       <c r="A133">
+        <v>3.16</v>
+      </c>
+      <c r="B133">
         <v>201503</v>
-      </c>
-      <c r="B133">
-        <v>3.16</v>
       </c>
       <c r="C133">
         <v>3.29</v>
@@ -3027,10 +3027,10 @@
     </row>
     <row r="134" spans="1:7">
       <c r="A134">
+        <v>3.14</v>
+      </c>
+      <c r="B134">
         <v>201504</v>
-      </c>
-      <c r="B134">
-        <v>3.14</v>
       </c>
       <c r="C134">
         <v>3.16</v>
@@ -3050,10 +3050,10 @@
     </row>
     <row r="135" spans="1:7">
       <c r="A135">
+        <v>3.06</v>
+      </c>
+      <c r="B135">
         <v>201505</v>
-      </c>
-      <c r="B135">
-        <v>3.06</v>
       </c>
       <c r="C135">
         <v>3.14</v>
@@ -3073,10 +3073,10 @@
     </row>
     <row r="136" spans="1:7">
       <c r="A136">
+        <v>3.2</v>
+      </c>
+      <c r="B136">
         <v>201506</v>
-      </c>
-      <c r="B136">
-        <v>3.2</v>
       </c>
       <c r="C136">
         <v>3.06</v>
@@ -3096,10 +3096,10 @@
     </row>
     <row r="137" spans="1:7">
       <c r="A137">
+        <v>3.07</v>
+      </c>
+      <c r="B137">
         <v>201507</v>
-      </c>
-      <c r="B137">
-        <v>3.07</v>
       </c>
       <c r="C137">
         <v>3.2</v>
@@ -3119,10 +3119,10 @@
     </row>
     <row r="138" spans="1:7">
       <c r="A138">
+        <v>3.11</v>
+      </c>
+      <c r="B138">
         <v>201508</v>
-      </c>
-      <c r="B138">
-        <v>3.11</v>
       </c>
       <c r="C138">
         <v>3.07</v>
@@ -3142,10 +3142,10 @@
     </row>
     <row r="139" spans="1:7">
       <c r="A139">
+        <v>3.17</v>
+      </c>
+      <c r="B139">
         <v>201509</v>
-      </c>
-      <c r="B139">
-        <v>3.17</v>
       </c>
       <c r="C139">
         <v>3.11</v>
@@ -3165,10 +3165,10 @@
     </row>
     <row r="140" spans="1:7">
       <c r="A140">
+        <v>3.14</v>
+      </c>
+      <c r="B140">
         <v>201510</v>
-      </c>
-      <c r="B140">
-        <v>3.14</v>
       </c>
       <c r="C140">
         <v>3.17</v>
@@ -3188,10 +3188,10 @@
     </row>
     <row r="141" spans="1:7">
       <c r="A141">
+        <v>3.01</v>
+      </c>
+      <c r="B141">
         <v>201511</v>
-      </c>
-      <c r="B141">
-        <v>3.01</v>
       </c>
       <c r="C141">
         <v>3.14</v>
@@ -3211,10 +3211,10 @@
     </row>
     <row r="142" spans="1:7">
       <c r="A142">
+        <v>3.01</v>
+      </c>
+      <c r="B142">
         <v>201512</v>
-      </c>
-      <c r="B142">
-        <v>3.01</v>
       </c>
       <c r="C142">
         <v>3.01</v>
@@ -3234,10 +3234,10 @@
     </row>
     <row r="143" spans="1:7">
       <c r="A143">
+        <v>2.93</v>
+      </c>
+      <c r="B143">
         <v>201601</v>
-      </c>
-      <c r="B143">
-        <v>2.93</v>
       </c>
       <c r="C143">
         <v>3.01</v>
@@ -3257,10 +3257,10 @@
     </row>
     <row r="144" spans="1:7">
       <c r="A144">
+        <v>2.83</v>
+      </c>
+      <c r="B144">
         <v>201602</v>
-      </c>
-      <c r="B144">
-        <v>2.83</v>
       </c>
       <c r="C144">
         <v>2.93</v>
@@ -3280,10 +3280,10 @@
     </row>
     <row r="145" spans="1:7">
       <c r="A145">
+        <v>2.91</v>
+      </c>
+      <c r="B145">
         <v>201603</v>
-      </c>
-      <c r="B145">
-        <v>2.91</v>
       </c>
       <c r="C145">
         <v>2.83</v>
@@ -3303,10 +3303,10 @@
     </row>
     <row r="146" spans="1:7">
       <c r="A146">
+        <v>2.93</v>
+      </c>
+      <c r="B146">
         <v>201604</v>
-      </c>
-      <c r="B146">
-        <v>2.93</v>
       </c>
       <c r="C146">
         <v>2.91</v>
@@ -3326,10 +3326,10 @@
     </row>
     <row r="147" spans="1:7">
       <c r="A147">
+        <v>2.99</v>
+      </c>
+      <c r="B147">
         <v>201605</v>
-      </c>
-      <c r="B147">
-        <v>2.99</v>
       </c>
       <c r="C147">
         <v>2.93</v>
@@ -3349,10 +3349,10 @@
     </row>
     <row r="148" spans="1:7">
       <c r="A148">
+        <v>2.94</v>
+      </c>
+      <c r="B148">
         <v>201606</v>
-      </c>
-      <c r="B148">
-        <v>2.94</v>
       </c>
       <c r="C148">
         <v>2.99</v>
@@ -3372,10 +3372,10 @@
     </row>
     <row r="149" spans="1:7">
       <c r="A149">
+        <v>2.8</v>
+      </c>
+      <c r="B149">
         <v>201607</v>
-      </c>
-      <c r="B149">
-        <v>2.8</v>
       </c>
       <c r="C149">
         <v>2.94</v>
@@ -3395,10 +3395,10 @@
     </row>
     <row r="150" spans="1:7">
       <c r="A150">
+        <v>2.86</v>
+      </c>
+      <c r="B150">
         <v>201608</v>
-      </c>
-      <c r="B150">
-        <v>2.86</v>
       </c>
       <c r="C150">
         <v>2.8</v>
@@ -3418,10 +3418,10 @@
     </row>
     <row r="151" spans="1:7">
       <c r="A151">
+        <v>2.92</v>
+      </c>
+      <c r="B151">
         <v>201609</v>
-      </c>
-      <c r="B151">
-        <v>2.92</v>
       </c>
       <c r="C151">
         <v>2.86</v>
@@ -3441,10 +3441,10 @@
     </row>
     <row r="152" spans="1:7">
       <c r="A152">
+        <v>2.75</v>
+      </c>
+      <c r="B152">
         <v>201610</v>
-      </c>
-      <c r="B152">
-        <v>2.75</v>
       </c>
       <c r="C152">
         <v>2.92</v>
@@ -3464,10 +3464,10 @@
     </row>
     <row r="153" spans="1:7">
       <c r="A153">
+        <v>2.7</v>
+      </c>
+      <c r="B153">
         <v>201611</v>
-      </c>
-      <c r="B153">
-        <v>2.7</v>
       </c>
       <c r="C153">
         <v>2.75</v>
@@ -3487,10 +3487,10 @@
     </row>
     <row r="154" spans="1:7">
       <c r="A154">
+        <v>2.68</v>
+      </c>
+      <c r="B154">
         <v>201612</v>
-      </c>
-      <c r="B154">
-        <v>2.68</v>
       </c>
       <c r="C154">
         <v>2.7</v>
@@ -3510,10 +3510,10 @@
     </row>
     <row r="155" spans="1:7">
       <c r="A155">
+        <v>2.71</v>
+      </c>
+      <c r="B155">
         <v>201701</v>
-      </c>
-      <c r="B155">
-        <v>2.71</v>
       </c>
       <c r="C155">
         <v>2.68</v>
@@ -3533,10 +3533,10 @@
     </row>
     <row r="156" spans="1:7">
       <c r="A156">
+        <v>2.73</v>
+      </c>
+      <c r="B156">
         <v>201702</v>
-      </c>
-      <c r="B156">
-        <v>2.73</v>
       </c>
       <c r="C156">
         <v>2.71</v>
@@ -3556,10 +3556,10 @@
     </row>
     <row r="157" spans="1:7">
       <c r="A157">
+        <v>2.84</v>
+      </c>
+      <c r="B157">
         <v>201703</v>
-      </c>
-      <c r="B157">
-        <v>2.84</v>
       </c>
       <c r="C157">
         <v>2.73</v>
@@ -3579,10 +3579,10 @@
     </row>
     <row r="158" spans="1:7">
       <c r="A158">
+        <v>2.83</v>
+      </c>
+      <c r="B158">
         <v>201704</v>
-      </c>
-      <c r="B158">
-        <v>2.83</v>
       </c>
       <c r="C158">
         <v>2.84</v>
@@ -3602,10 +3602,10 @@
     </row>
     <row r="159" spans="1:7">
       <c r="A159">
+        <v>2.86</v>
+      </c>
+      <c r="B159">
         <v>201705</v>
-      </c>
-      <c r="B159">
-        <v>2.86</v>
       </c>
       <c r="C159">
         <v>2.83</v>
@@ -3625,10 +3625,10 @@
     </row>
     <row r="160" spans="1:7">
       <c r="A160">
+        <v>2.95</v>
+      </c>
+      <c r="B160">
         <v>201706</v>
-      </c>
-      <c r="B160">
-        <v>2.95</v>
       </c>
       <c r="C160">
         <v>2.86</v>
@@ -3648,10 +3648,10 @@
     </row>
     <row r="161" spans="1:7">
       <c r="A161">
+        <v>2.99</v>
+      </c>
+      <c r="B161">
         <v>201707</v>
-      </c>
-      <c r="B161">
-        <v>2.99</v>
       </c>
       <c r="C161">
         <v>2.95</v>
@@ -3671,10 +3671,10 @@
     </row>
     <row r="162" spans="1:7">
       <c r="A162">
+        <v>3.06</v>
+      </c>
+      <c r="B162">
         <v>201708</v>
-      </c>
-      <c r="B162">
-        <v>3.06</v>
       </c>
       <c r="C162">
         <v>2.99</v>
@@ -3694,10 +3694,10 @@
     </row>
     <row r="163" spans="1:7">
       <c r="A163">
+        <v>3.08</v>
+      </c>
+      <c r="B163">
         <v>201709</v>
-      </c>
-      <c r="B163">
-        <v>3.08</v>
       </c>
       <c r="C163">
         <v>3.06</v>
@@ -3717,10 +3717,10 @@
     </row>
     <row r="164" spans="1:7">
       <c r="A164">
+        <v>3.12</v>
+      </c>
+      <c r="B164">
         <v>201710</v>
-      </c>
-      <c r="B164">
-        <v>3.12</v>
       </c>
       <c r="C164">
         <v>3.08</v>
@@ -3740,10 +3740,10 @@
     </row>
     <row r="165" spans="1:7">
       <c r="A165">
+        <v>3.08</v>
+      </c>
+      <c r="B165">
         <v>201711</v>
-      </c>
-      <c r="B165">
-        <v>3.08</v>
       </c>
       <c r="C165">
         <v>3.12</v>
@@ -3763,10 +3763,10 @@
     </row>
     <row r="166" spans="1:7">
       <c r="A166">
+        <v>3.14</v>
+      </c>
+      <c r="B166">
         <v>201712</v>
-      </c>
-      <c r="B166">
-        <v>3.14</v>
       </c>
       <c r="C166">
         <v>3.08</v>
@@ -3786,10 +3786,10 @@
     </row>
     <row r="167" spans="1:7">
       <c r="A167">
+        <v>3.09</v>
+      </c>
+      <c r="B167">
         <v>201801</v>
-      </c>
-      <c r="B167">
-        <v>3.09</v>
       </c>
       <c r="C167">
         <v>3.14</v>
@@ -3809,10 +3809,10 @@
     </row>
     <row r="168" spans="1:7">
       <c r="A168">
+        <v>3.29</v>
+      </c>
+      <c r="B168">
         <v>201802</v>
-      </c>
-      <c r="B168">
-        <v>3.29</v>
       </c>
       <c r="C168">
         <v>3.09</v>
@@ -3832,10 +3832,10 @@
     </row>
     <row r="169" spans="1:7">
       <c r="A169">
+        <v>3.26</v>
+      </c>
+      <c r="B169">
         <v>201803</v>
-      </c>
-      <c r="B169">
-        <v>3.26</v>
       </c>
       <c r="C169">
         <v>3.29</v>
@@ -3855,10 +3855,10 @@
     </row>
     <row r="170" spans="1:7">
       <c r="A170">
+        <v>3.23</v>
+      </c>
+      <c r="B170">
         <v>201804</v>
-      </c>
-      <c r="B170">
-        <v>3.23</v>
       </c>
       <c r="C170">
         <v>3.26</v>
@@ -3878,10 +3878,10 @@
     </row>
     <row r="171" spans="1:7">
       <c r="A171">
+        <v>3.21</v>
+      </c>
+      <c r="B171">
         <v>201805</v>
-      </c>
-      <c r="B171">
-        <v>3.21</v>
       </c>
       <c r="C171">
         <v>3.23</v>
@@ -3901,10 +3901,10 @@
     </row>
     <row r="172" spans="1:7">
       <c r="A172">
+        <v>3.13</v>
+      </c>
+      <c r="B172">
         <v>201806</v>
-      </c>
-      <c r="B172">
-        <v>3.13</v>
       </c>
       <c r="C172">
         <v>3.21</v>
@@ -3924,10 +3924,10 @@
     </row>
     <row r="173" spans="1:7">
       <c r="A173">
+        <v>3.13</v>
+      </c>
+      <c r="B173">
         <v>201807</v>
-      </c>
-      <c r="B173">
-        <v>3.13</v>
       </c>
       <c r="C173">
         <v>3.13</v>

</xml_diff>